<commit_message>
update fsl_quality and cleaning
</commit_message>
<xml_diff>
--- a/inst/fsl_quality_report/resources/flag_description.xlsx
+++ b/inst/fsl_quality_report/resources/flag_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\IPHRA_toolkit\cleaning\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\fsl_quality_report\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688B33F7-C545-4314-91D9-91FBB54A4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8496E1-EEA1-460B-B96D-4F7C4D15FB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSL" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>If high SD, FCS entries to be reviewed for enumerator bias at beginning of data collection.</t>
   </si>
   <si>
-    <t>flag_SD_foodgroups</t>
-  </si>
-  <si>
     <t>Script calculates 'sd_foodgroups' measuring the standard deviation among food groups entries. If sd_foodgroups is lower than 0.8, high descrepencies among the FCS entry should be flagged. Repetitive entry (5,4,5,4,5,…), all high (fcs =112) or all low (fcs = 0) entries should be reviewed for enumerator bias.</t>
   </si>
   <si>
@@ -458,6 +455,9 @@
   </si>
   <si>
     <t>Respondent reported sex of dead person male and a cause of death related to female only.</t>
+  </si>
+  <si>
+    <t>flag_sd_foodgroup</t>
   </si>
 </sst>
 </file>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,400 +844,400 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
         <v>69</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>72</v>
-      </c>
-      <c r="C26" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>81</v>
-      </c>
-      <c r="C29" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>84</v>
-      </c>
-      <c r="C30" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
-        <v>87</v>
-      </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
         <v>88</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
         <v>91</v>
-      </c>
-      <c r="B33" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
         <v>98</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>99</v>
-      </c>
-      <c r="C36" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" t="s">
         <v>101</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>102</v>
-      </c>
-      <c r="C37" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
         <v>104</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
         <v>107</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>108</v>
-      </c>
-      <c r="C39" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" t="s">
         <v>110</v>
-      </c>
-      <c r="B40" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
         <v>112</v>
-      </c>
-      <c r="B41" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
         <v>114</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>115</v>
-      </c>
-      <c r="C42" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1272,68 +1272,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
         <v>124</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
         <v>129</v>
-      </c>
-      <c r="C6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1368,35 +1368,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
       </c>
-      <c r="B2" t="s">
-        <v>133</v>
-      </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
         <v>135</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>136</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8440C440-E586-4116-9669-C7C58F9A3DB2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1431,24 +1431,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the fsl_flag_desctiption file
</commit_message>
<xml_diff>
--- a/inst/fsl_quality_report/resources/flag_description.xlsx
+++ b/inst/fsl_quality_report/resources/flag_description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\fsl_quality_report\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8496E1-EEA1-460B-B96D-4F7C4D15FB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99CAD8E-D475-4550-8A3A-35FA726728F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="144">
   <si>
     <t>flag_name</t>
   </si>
@@ -87,9 +87,6 @@
     <t xml:space="preserve">In many contexty, types of fat are commonly used for meal preparation, along with cereals as basic staples. </t>
   </si>
   <si>
-    <t xml:space="preserve">If reported consumption is low, review according to food sources and livelihoods sytems for coherence. </t>
-  </si>
-  <si>
     <t>flag_low_oil</t>
   </si>
   <si>
@@ -99,18 +96,12 @@
     <t>flag_low_fcs</t>
   </si>
   <si>
-    <t>Except if in EXTREME cases (e.g. Somalia), it will be very rare for many/any HHs to have such low FCS scores</t>
-  </si>
-  <si>
     <t>Review with enumerators if corresponds to observed vulneraiblity of households and flag to PHU</t>
   </si>
   <si>
     <t>flag_high_fcs</t>
   </si>
   <si>
-    <t>FCS total score is 112 which corresponds to consuming all food groups every day, highly unlikely in any context. WFP set threshold starting from 56 considered already has high. To be reviewed against context for coherence.</t>
-  </si>
-  <si>
     <t>Review with enumerators if corresponds to observed vulneraiblity of households</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>flag_fcs_rcsi</t>
   </si>
   <si>
-    <t>FCS and rCSI are strongly correlated with a negative relation. This combination is't impossible but needs to be verified within its context. If collected in early stages of a crisis, would be expected that rCSI will still be sensitive enough to measure early consumption-based coping and measure a higher score.</t>
-  </si>
-  <si>
     <t>Review based on context and crisis stage, whether not engaging in consumption-based coping would be linked to exhaustion of these strategies (in a protracted context) or to issues in collecting this data in the correct way.</t>
   </si>
   <si>
@@ -153,9 +141,6 @@
     <t>flag_protein_rcsi</t>
   </si>
   <si>
-    <t xml:space="preserve">If rCSI score is high (in contexts of early crisis stages) while protein consumption is also reported as frequent ( min. 5 days), it could be that either dimension wasn't understood or collected properly. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Review with enumerators teams if consumption-based coping were really applied because of lack of food, and/or well understood (review frequency) AND/OR review which protein are mainly reported: meat, chicken or eggs? Depending on the livelihood system or market prices, high protein consumption could be explained but if not (HH doesn't appear to own livestock for instance), remove rCSI entry if other food groups are also frequently consumed in line with local dietary patterns.  </t>
   </si>
   <si>
@@ -198,9 +183,6 @@
     <t>flag_severe_hhs</t>
   </si>
   <si>
-    <t xml:space="preserve">reports of severe and very severe hunger are flags for particularly At Risk Households suffering from prolonged acute food insecurity </t>
-  </si>
-  <si>
     <t>Flag to PHU team</t>
   </si>
   <si>
@@ -292,9 +274,6 @@
   </si>
   <si>
     <t>flag_fcsrcsi_box</t>
-  </si>
-  <si>
-    <t>Any HH that would have an acceptable FCS score (higher scores) and a high rCSI score is most likely indicative of data quality issue with one or both indicators</t>
   </si>
   <si>
     <t>Review both FCS and rCSI entries with concerned enumerators</t>
@@ -458,16 +437,46 @@
   </si>
   <si>
     <t>flag_sd_foodgroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If reported oil consumption is low (oill&lt;5 days), review according to food sources and livelihoods sytems for coherence. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If reported cereal consumption is low (cereal&lt;5 days), review according to food sources and livelihoods sytems for coherence. </t>
+  </si>
+  <si>
+    <t>Except if in EXTREME cases (e.g. Somalia), it will be very rare for many/any HHs to have such low FCS scores (FCS &lt;10)</t>
+  </si>
+  <si>
+    <t>FCS total score is 112 which corresponds to consuming all food groups every day, highly unlikely in any context. WFP considered FCS&gt;56 already as high. To be reviewed against context for coherence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If fcs_score &lt; 35 and rcsi_score &lt;= 4. FCS and rCSI are strongly correlated with a negative relation. This combination is't impossible but needs to be verified within its context. If collected in early stages of a crisis, would be expected that rCSI will still be sensitive enough to measure early consumption-based coping and measure a higher score.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If rCSI score is high (in contexts of early crisis stages) while protein consumption is also reported as frequent (min. 5 days), it could be that either dimension wasn't understood or collected properly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If HHS score &gt;= 5. Reports of severe and very severe hunger are flags for particularly At Risk Households suffering from prolonged acute food insecurity </t>
+  </si>
+  <si>
+    <t>If HH has both rCSI score&gt;18 and FCS score&gt;56. Any HH that would have an acceptable FCS score (higher scores) and a high rCSI score is most likely indicative of data quality issue with one or both indicators</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,8 +502,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,467 +787,468 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="120.7109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="120.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="C27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B35" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C35" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C36" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B37" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B38" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B40" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C38" t="s">
+      <c r="B41" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1272,68 +1283,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
         <v>117</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
         <v>118</v>
       </c>
-      <c r="B3" t="s">
-        <v>125</v>
-      </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
         <v>119</v>
       </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
         <v>120</v>
       </c>
-      <c r="B5" t="s">
-        <v>127</v>
-      </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
         <v>121</v>
       </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1368,35 +1379,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1431,24 +1442,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>